<commit_message>
new item for refine
</commit_message>
<xml_diff>
--- a/plan/excel/item_道具表.xlsx
+++ b/plan/excel/item_道具表.xlsx
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="72">
   <si>
     <t>number</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -453,6 +453,22 @@
   </si>
   <si>
     <t>icon/item/item_4105.png</t>
+  </si>
+  <si>
+    <t>精炼符</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级精炼符</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon/item/item_4111.png</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon/item/item_4112.png</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -840,11 +856,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1417,6 +1433,78 @@
         <v>0</v>
       </c>
       <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>4111</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>4112</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
         <v>0</v>
       </c>
     </row>

</xml_diff>